<commit_message>
Completed list of matches
</commit_message>
<xml_diff>
--- a/7thGameWTA.xlsx
+++ b/7thGameWTA.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C107"/>
+  <dimension ref="A1:C105"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,1802 +446,1768 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ATP Belgrade 2</t>
+          <t>Adelaide</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/belgrade-2/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/adelaide/</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/belgrade-2/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/adelaide/results/</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ATP Finals - Turin</t>
+          <t>Amersfoort</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/finals-turin/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/amersfoort/</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/finals-turin/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/amersfoort/results/</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ATP Metz</t>
+          <t>Antalya</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/metz/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/antalya/</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/metz/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/antalya/results/</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Adelaide</t>
+          <t>Antwerp</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/adelaide/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/antwerp/</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/adelaide/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/antwerp/results/</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Amersfoort</t>
+          <t>ATP Cup</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/amersfoort/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/atp-cup/</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/amersfoort/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/atp-cup/results/</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Antalya</t>
+          <t>Auckland</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/antalya/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/auckland/</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/antalya/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/auckland/results/</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Antwerp</t>
+          <t>Australian Open</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/antwerp/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/australian-open/</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/antwerp/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/australian-open/results/</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>ATP Cup</t>
+          <t>Bangkok</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/atp-cup/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/bangkok/</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/atp-cup/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/bangkok/results/</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Auckland</t>
+          <t>Barcelona</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/auckland/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/barcelona/</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/auckland/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/barcelona/results/</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Australian Open</t>
+          <t>Basel</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/australian-open/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/basel/</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/australian-open/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/basel/results/</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Bangkok</t>
+          <t>Bastad</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/bangkok/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/bastad/</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/bangkok/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/bastad/results/</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Barcelona</t>
+          <t>Beijing</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/barcelona/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/beijing/</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/barcelona/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/beijing/results/</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Basel</t>
+          <t>Belgrade</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/basel/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/belgrade/</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/basel/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/belgrade/results/</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Bastad</t>
+          <t>Bogota</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/bastad/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/bogota/</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/bastad/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/bogota/results/</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Beijing</t>
+          <t>Brisbane</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/beijing/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/brisbane/</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/beijing/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/brisbane/results/</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Belgrade</t>
+          <t>Budapest</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/belgrade/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/budapest/</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/belgrade/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/budapest/results/</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Bogota</t>
+          <t>Buenos Aires</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/bogota/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/buenos-aires/</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/bogota/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/buenos-aires/results/</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Brisbane</t>
+          <t>Casablanca</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/brisbane/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/casablanca/</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/brisbane/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/casablanca/results/</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Budapest</t>
+          <t>Chengdu</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/budapest/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/chengdu/</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/budapest/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/chengdu/results/</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Buenos Aires</t>
+          <t>Chennai</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/buenos-aires/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/chennai/</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/buenos-aires/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/chennai/results/</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Casablanca</t>
+          <t>Copenhagen</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/casablanca/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/copenhagen/</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/casablanca/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/copenhagen/results/</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Chengdu</t>
+          <t>Cordoba</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/chengdu/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/cordoba/</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/chengdu/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/cordoba/results/</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Chennai</t>
+          <t>Costa Do Sauipe</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/chennai/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/costa-do-sauipe/</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/chennai/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/costa-do-sauipe/results/</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Copenhagen</t>
+          <t>Davis Cup - World Group</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/copenhagen/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/davis-cup-world-group/</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/copenhagen/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/davis-cup-world-group/results/</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Cordoba</t>
+          <t>Doha</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/cordoba/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/doha/</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/cordoba/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/doha/results/</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Costa Do Sauipe</t>
+          <t>Dubai</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/costa-do-sauipe/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/dubai/</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/costa-do-sauipe/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/dubai/results/</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Davis Cup - World Group</t>
+          <t>Dusseldorf</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/davis-cup-world-group/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/dusseldorf/</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/davis-cup-world-group/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/dusseldorf/results/</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Doha</t>
+          <t>Eastbourne</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/doha/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/eastbourne/</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/doha/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/eastbourne/results/</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Dubai</t>
+          <t>Estoril</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/dubai/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/estoril/</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/dubai/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/estoril/results/</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Dusseldorf</t>
+          <t>Finals - Turin</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/dusseldorf/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/finals-turin/</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/dusseldorf/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/finals-turin/results/</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Eastbourne</t>
+          <t>French Open</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/eastbourne/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/french-open/</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/eastbourne/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/french-open/results/</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Estoril</t>
+          <t>Geneva</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/estoril/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/geneva/</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/estoril/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/geneva/results/</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Finals - Turin</t>
+          <t>Gstaad</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/finals-turin/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/gstaad/</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/finals-turin/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/gstaad/results/</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>French Open</t>
+          <t>Halle</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/french-open/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/halle/</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/french-open/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/halle/results/</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Geneva</t>
+          <t>Hamburg</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/geneva/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/hamburg/</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/geneva/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/hamburg/results/</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Gstaad</t>
+          <t>Ho Chi Minh City</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/gstaad/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/ho-chi-minh-city/</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/gstaad/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/ho-chi-minh-city/results/</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Halle</t>
+          <t>Hong Kong</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/halle/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/hong-kong/</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/halle/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/hong-kong/results/</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Hamburg</t>
+          <t>Houston</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/hamburg/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/houston/</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/hamburg/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/houston/results/</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Ho Chi Minh City</t>
+          <t>Indianapolis</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/ho-chi-minh-city/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/indianapolis/</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/ho-chi-minh-city/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/indianapolis/results/</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Hong Kong</t>
+          <t>Istanbul</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/hong-kong/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/istanbul/</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/hong-kong/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/istanbul/results/</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Kitzbuhel</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/houston/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/kitzbuhel/</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/houston/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/kitzbuhel/results/</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Indianapolis</t>
+          <t>Kuala Lumpur</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/indianapolis/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/kuala-lumpur/</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/indianapolis/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/kuala-lumpur/results/</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Istanbul</t>
+          <t>Las Vegas</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/istanbul/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/las-vegas/</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/istanbul/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/las-vegas/results/</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Kitzbuhel</t>
+          <t>Laver Cup</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/kitzbuhel/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/laver-cup/</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/kitzbuhel/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/laver-cup/results/</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Kuala Lumpur</t>
+          <t>London</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/kuala-lumpur/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/london/</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/kuala-lumpur/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/london/results/</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Las Vegas</t>
+          <t>Long Island</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/las-vegas/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/long-island/</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/las-vegas/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/long-island/results/</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Laver Cup</t>
+          <t>Los Angeles</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/laver-cup/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/los-angeles/</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/laver-cup/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/los-angeles/results/</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>London</t>
+          <t>Los Cabos</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/london/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/los-cabos/</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/london/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/los-cabos/results/</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Long Island</t>
+          <t>Lyon</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/long-island/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/lyon/</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/long-island/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/lyon/results/</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Los Angeles</t>
+          <t>Madrid</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/los-angeles/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/madrid/</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/los-angeles/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/madrid/results/</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Los Cabos</t>
+          <t>Mallorca</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/los-cabos/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/mallorca/</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/los-cabos/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/mallorca/results/</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Lyon</t>
+          <t>Marrakech</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/lyon/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/marrakech/</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/lyon/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/marrakech/results/</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Madrid</t>
+          <t>Marseille</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/madrid/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/marseille/</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/madrid/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/marseille/results/</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Mallorca</t>
+          <t>Memphis</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/mallorca/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/memphis/</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/mallorca/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/memphis/results/</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Marrakech</t>
+          <t>Metz</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/marrakech/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/metz/</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/marrakech/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/metz/results/</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Marseille</t>
+          <t>Miami</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/marseille/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/miami/</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/marseille/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/miami/results/</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>Milan</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/memphis/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/milan/</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/memphis/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/milan/results/</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Metz</t>
+          <t>Monte Carlo</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/metz/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/monte-carlo/</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/metz/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/monte-carlo/results/</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Montpellier</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/miami/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/montpellier/</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/miami/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/montpellier/results/</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Milan</t>
+          <t>Montreal</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/milan/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/montreal/</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/milan/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/montreal/results/</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Monte Carlo</t>
+          <t>Moscow</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/monte-carlo/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/moscow/</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/monte-carlo/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/moscow/results/</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Montpellier</t>
+          <t>Mumbai</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/montpellier/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/mumbai/</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/montpellier/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/mumbai/results/</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Montreal</t>
+          <t>Munich</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/montreal/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/munich/</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/montreal/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/munich/results/</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Moscow</t>
+          <t>New Haven</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/moscow/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/new-haven/</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/moscow/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/new-haven/results/</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Mumbai</t>
+          <t>Newport</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/mumbai/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/newport/</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/mumbai/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/newport/results/</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Munich</t>
+          <t>Next Gen Finals - Jeddah</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/munich/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/next-gen-finals-jeddah/</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/munich/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/next-gen-finals-jeddah/results/</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>New Haven</t>
+          <t>Nice</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/new-haven/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/nice/</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/new-haven/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/nice/results/</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Newport</t>
+          <t>Nottingham</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/newport/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/nottingham/</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/newport/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/nottingham/results/</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Next Gen Finals - Jeddah</t>
+          <t>Olympic Games</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/next-gen-finals-jeddah/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/olympic-games/</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/next-gen-finals-jeddah/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/olympic-games/results/</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Nice</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/nice/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/palermo/</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/nice/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/palermo/results/</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Nottingham</t>
+          <t>Paris</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/nottingham/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/paris/</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/nottingham/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/paris/results/</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Olympic Games</t>
+          <t>Poertschach</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/olympic-games/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/poertschach/</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/olympic-games/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/poertschach/results/</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Pune</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/palermo/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/pune/</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/palermo/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/pune/results/</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Paris</t>
+          <t>Quito</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/paris/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/quito/</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/paris/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/quito/results/</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Poertschach</t>
+          <t>Rio de Janeiro</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/poertschach/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/rio-de-janeiro/</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/poertschach/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/rio-de-janeiro/results/</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Pune</t>
+          <t>Rome</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/pune/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/rome/</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/pune/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/rome/results/</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Quito</t>
+          <t>Rotterdam</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/quito/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/rotterdam/</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/quito/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/rotterdam/results/</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Rio de Janeiro</t>
+          <t>San Jose</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/rio-de-janeiro/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/san-jose/</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/rio-de-janeiro/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/san-jose/results/</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Rome</t>
+          <t>Santiago</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/rome/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/santiago/</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/rome/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/santiago/results/</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Rotterdam</t>
+          <t>Sao Paulo</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/rotterdam/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/sao-paulo/</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/rotterdam/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/sao-paulo/results/</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>San Jose</t>
+          <t>Scottsdale</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/san-jose/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/scottsdale/</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/san-jose/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/scottsdale/results/</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Santiago</t>
+          <t>Shanghai</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/santiago/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/shanghai/</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/santiago/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/shanghai/results/</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Sao Paulo</t>
+          <t>Shenzhen</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/sao-paulo/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/shenzhen/</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/sao-paulo/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/shenzhen/results/</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Scottsdale</t>
+          <t>Sofia</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/scottsdale/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/sofia/</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/scottsdale/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/sofia/results/</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Shanghai</t>
+          <t>Sopot</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/shanghai/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/sopot/</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/shanghai/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/sopot/results/</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Shenzhen</t>
+          <t>Stockholm</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/shenzhen/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/stockholm/</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/shenzhen/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/stockholm/results/</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Sofia</t>
+          <t>St. Petersburg</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/sofia/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/st-petersburg/</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/sofia/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/st-petersburg/results/</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Sopot</t>
+          <t>Stuttgart</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/sopot/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/stuttgart/</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/sopot/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/stuttgart/results/</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Stockholm</t>
+          <t>Sydney</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/stockholm/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/sydney/</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/stockholm/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/sydney/results/</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>St. Petersburg</t>
+          <t>Tashkent</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/st-petersburg/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/tashkent/</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/st-petersburg/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/tashkent/results/</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Stuttgart</t>
+          <t>Tel Aviv</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/stuttgart/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/tel-aviv/</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/stuttgart/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/tel-aviv/results/</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>Tokyo</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/sydney/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/tokyo/</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/sydney/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/tokyo/results/</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Tashkent</t>
+          <t>Toronto</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/tashkent/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/toronto/</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/tashkent/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/toronto/results/</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Tel Aviv</t>
+          <t>US Open</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/tel-aviv/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/us-open/</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/tel-aviv/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/us-open/results/</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Tokyo</t>
+          <t>Valencia</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/tokyo/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/valencia/</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/tokyo/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/valencia/results/</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Toronto</t>
+          <t>Vienna</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/toronto/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/vienna/</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/toronto/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/vienna/results/</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>US Open</t>
+          <t>Vina del Mar</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/us-open/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/vina-del-mar/</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/us-open/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/vina-del-mar/results/</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Valencia</t>
+          <t>Warsaw</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/valencia/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/warsaw/</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/valencia/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/warsaw/results/</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Vienna</t>
+          <t>Washington</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/vienna/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/washington/</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/vienna/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/washington/results/</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Vina del Mar</t>
+          <t>Wimbledon</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/vina-del-mar/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/wimbledon/</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/vina-del-mar/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/wimbledon/results/</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Warsaw</t>
+          <t>Winston-Salem</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/warsaw/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/winston-salem/</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/warsaw/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/winston-salem/results/</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Washington</t>
+          <t>Zhuhai</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/washington/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/zhuhai/</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/washington/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/zhuhai/results/</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Wimbledon</t>
+          <t>ATP Australian Open</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/wimbledon/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/australian-open/</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/wimbledon/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/australian-open/results/</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Winston-Salem</t>
+          <t>ATP Wimbledon</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/winston-salem/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/wimbledon/</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>https://www.livesport.com/tennis/atp-singles/winston-salem/results/</t>
-        </is>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="inlineStr">
-        <is>
-          <t>Zhuhai</t>
-        </is>
-      </c>
-      <c r="B106" t="inlineStr">
-        <is>
-          <t>https://www.livesport.com/tennis/atp-singles/zhuhai/</t>
-        </is>
-      </c>
-      <c r="C106" t="inlineStr">
-        <is>
-          <t>https://www.livesport.com/tennis/atp-singles/zhuhai/results/</t>
-        </is>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" t="inlineStr">
-        <is>
-          <t>ATP Australian Open</t>
-        </is>
-      </c>
-      <c r="B107" t="inlineStr">
-        <is>
-          <t>https://www.livesport.com/tennis/atp-singles/australian-open/</t>
-        </is>
-      </c>
-      <c r="C107" t="inlineStr">
-        <is>
-          <t>https://www.livesport.com/tennis/atp-singles/australian-open/results/</t>
+          <t>https://www.livesport.com/tennis/atp-singles/wimbledon/results/</t>
         </is>
       </c>
     </row>
@@ -2455,10 +2421,6 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C104" r:id="rId206"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B105" r:id="rId207"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C105" r:id="rId208"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B106" r:id="rId209"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C106" r:id="rId210"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B107" r:id="rId211"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C107" r:id="rId212"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>